<commit_message>
Final changes in Array
</commit_message>
<xml_diff>
--- a/testData/Python_Editor_Data.xlsx
+++ b/testData/Python_Editor_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NumpyNinja\NN_DS_Algo\DS_ALGO_August_Currently Working\NN_DS_ALGO_SDET-WARRIORS\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A1DA7D-4889-43DA-8739-B4D784913879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55E68F3-C2A4-4B62-8C8F-1539DD6355E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{E0E5FE83-F7EC-4FA9-ABD6-F2830CC9D99A}"/>
   </bookViews>
@@ -548,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86300902-3A55-4EDA-8E85-80F249BBB131}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,7 +639,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="309.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="296.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>